<commit_message>
att slide final @brunagd
</commit_message>
<xml_diff>
--- a/Documentação/Riscos.xlsx
+++ b/Documentação/Riscos.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bunag\Desktop\control-block\Documentação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Desktop\control-block\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C54A3C-B117-4D7F-829B-9ED0C022E44E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="42">
   <si>
     <t>#</t>
   </si>
@@ -156,7 +155,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -227,7 +226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -257,6 +256,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -572,11 +574,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:P22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,10 +635,10 @@
       <c r="D3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="10">
         <v>4</v>
       </c>
       <c r="G3" s="7" t="s">
@@ -659,10 +661,10 @@
       <c r="D4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="9">
         <v>9</v>
       </c>
       <c r="G4" s="7" t="s">
@@ -685,10 +687,10 @@
       <c r="D5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="9">
         <v>6</v>
       </c>
       <c r="G5" s="7" t="s">
@@ -711,10 +713,10 @@
       <c r="D6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="9">
         <v>6</v>
       </c>
       <c r="G6" s="7" t="s">
@@ -737,10 +739,10 @@
       <c r="D7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="9">
         <v>6</v>
       </c>
       <c r="G7" s="7" t="s">
@@ -763,10 +765,10 @@
       <c r="D8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="9">
         <v>6</v>
       </c>
       <c r="G8" s="7" t="s">
@@ -789,10 +791,10 @@
       <c r="D9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="10">
         <v>3</v>
       </c>
       <c r="G9" s="7" t="s">
@@ -815,10 +817,10 @@
       <c r="D10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="10">
         <v>4</v>
       </c>
       <c r="G10" s="7" t="s">

</xml_diff>